<commit_message>
Está sendo possivel fazer pesquisas pelo assitente
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesgranatyr/Documents/Ensino/IA Expert/Cursos/Assistente Virtual/curso_assistente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzurlo\Downloads\Curso IA\Pycharm\Assistente_Virtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A90D01-A057-1B44-8367-E035914D9D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B5246A-E225-4E76-A0B4-656D80367B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="2220" windowWidth="15600" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,16 +378,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,12 +403,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>44911</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>45353</v>
       </c>
       <c r="B2" s="2">
-        <v>0.72916666666666663</v>
+        <v>0.95763888888888893</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -414,12 +417,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>44911</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>45353</v>
       </c>
       <c r="B3" s="2">
-        <v>0.75</v>
+        <v>0.95763888888888893</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -428,12 +431,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>44911</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>45353</v>
       </c>
       <c r="B4" s="2">
-        <v>0.79166666666666663</v>
+        <v>0.95763888888888893</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -442,23 +445,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
     </row>

</xml_diff>